<commit_message>
added comments and updated IOS community POM package
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testResults.xlsx
+++ b/Beton/src/main/resources/dataSheets/testResults.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="6">
   <si>
     <t>Test Parameters</t>
   </si>
@@ -77,8 +77,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -109,7 +115,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="1">
+      <c r="B2" t="s" s="7">
         <v>3</v>
       </c>
     </row>
@@ -117,7 +123,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" t="s" s="9">
         <v>3</v>
       </c>
     </row>
@@ -125,7 +131,7 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B4" t="s" s="12">
         <v>3</v>
       </c>
     </row>
@@ -159,7 +165,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="8">
         <v>3</v>
       </c>
     </row>
@@ -167,7 +173,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="10">
         <v>3</v>
       </c>
     </row>
@@ -175,7 +181,7 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="6">
+      <c r="B4" t="s" s="11">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added keyword driven basic and partial adapter
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testResults.xlsx
+++ b/Beton/src/main/resources/dataSheets/testResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="9">
   <si>
     <t>Test Parameters</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>googleTest</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -108,6 +111,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -163,12 +169,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="13">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -225,6 +240,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="15">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -245,7 +268,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="54.8359375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.6796875" collapsed="true"/>
-    <col min="3" max="3" width="10.6796875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.6796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -283,6 +306,14 @@
         <v>6</v>
       </c>
       <c r="C4" t="s" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="14">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Vzw keyword driven demo
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testResults.xlsx
+++ b/Beton/src/main/resources/dataSheets/testResults.xlsx
@@ -9,12 +9,13 @@
     <sheet name="Galaxy S5 SM-G900A ShirNate" r:id="rId3" sheetId="1"/>
     <sheet name="iPhone-6 Avner" r:id="rId4" sheetId="2"/>
     <sheet name="iPhone-6 Raj" r:id="rId5" sheetId="3"/>
+    <sheet name="null" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="9">
   <si>
     <t>Test Parameters</t>
   </si>
@@ -97,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -112,6 +113,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
@@ -244,7 +247,7 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s" s="15">
+      <c r="C5" t="s" s="17">
         <v>7</v>
       </c>
     </row>
@@ -253,6 +256,7 @@
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -313,7 +317,7 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s" s="14">
+      <c r="C5" t="s" s="16">
         <v>7</v>
       </c>
     </row>
@@ -322,7 +326,29 @@
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added support for screenshot as a link in the report
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testResults.xlsx
+++ b/Beton/src/main/resources/dataSheets/testResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="138">
   <si>
     <t>Test Parameters</t>
   </si>
@@ -864,6 +864,9 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>